<commit_message>
update test files. some validation changes
</commit_message>
<xml_diff>
--- a/tests/data/valid.mirri.xlsx
+++ b/tests/data/valid.mirri.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Geographic origin" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Strains" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sexual states" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sexual state" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Genomic information" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Markers" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Literature" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Growth media" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Ontobiotype" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Ontobiotope" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23661,7 +23661,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E79" activeCellId="2" sqref="AE2:AE20 AE21 E79"/>
+      <selection pane="topLeft" activeCell="E79" activeCellId="0" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25014,12 +25014,12 @@
   </sheetPr>
   <dimension ref="A1:AY21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE21" activeCellId="1" sqref="AE2:AE20 AE21"/>
+      <selection pane="bottomRight" activeCell="AE21" activeCellId="0" sqref="AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26580,8 +26580,8 @@
   </sheetPr>
   <dimension ref="A1:A241"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="AE2:AE20 AE21 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27810,7 +27810,7 @@
   <dimension ref="A1:D1016"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="2" sqref="AE2:AE20 AE21 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29970,7 +29970,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="AE2:AE20 AE21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30078,7 +30078,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="AE2:AE20 AE21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30143,7 +30143,7 @@
   <dimension ref="A1:C373"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A355" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="2" sqref="AE2:AE20 AE21 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30655,7 +30655,7 @@
   <dimension ref="A1:B3603"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="AE2:AE20 AE21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added script to upload data thow web services. Improve client and serializers
</commit_message>
<xml_diff>
--- a/tests/data/valid.mirri.xlsx
+++ b/tests/data/valid.mirri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Geographic origin" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8148" uniqueCount="7843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8146" uniqueCount="7843">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -24995,7 +24995,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -25010,12 +25010,12 @@
   </sheetPr>
   <dimension ref="A1:AY21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AJ1048526" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AJ1" activeCellId="0" sqref="AJ1"/>
-      <selection pane="bottomLeft" activeCell="A1048526" activeCellId="0" sqref="A1048526"/>
-      <selection pane="bottomRight" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AJ5" activeCellId="0" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26567,7 +26567,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27796,7 +27796,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29946,7 +29946,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30054,7 +30054,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30069,8 +30069,8 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30132,8 +30132,8 @@
       <c r="E2" s="0" t="s">
         <v>615</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>615</v>
+      <c r="F2" s="0" t="n">
+        <v>1991</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>615</v>
@@ -30161,8 +30161,8 @@
       <c r="E3" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>616</v>
+      <c r="F3" s="0" t="n">
+        <v>1992</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>616</v>
@@ -30177,7 +30177,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30689,7 +30689,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -59541,7 +59541,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
improvement and fixez in upload tool. Validation updated
</commit_message>
<xml_diff>
--- a/tests/data/valid.mirri.xlsx
+++ b/tests/data/valid.mirri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geographic origin" sheetId="1" state="visible" r:id="rId2"/>
@@ -25010,12 +25010,12 @@
   </sheetPr>
   <dimension ref="A1:AY21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AJ1" activeCellId="0" sqref="AJ1"/>
+      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ5" activeCellId="0" sqref="AJ5"/>
+      <selection pane="bottomRight" activeCell="W2" activeCellId="0" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30069,8 +30069,8 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>